<commit_message>
new report and log4J
</commit_message>
<xml_diff>
--- a/src/test/java/utility/testdata.xlsx
+++ b/src/test/java/utility/testdata.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{192E66D7-E9D1-45F1-82DF-35D8DAF0A764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2CF9C9C1-028B-4073-A573-F960C5284E15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4365" yWindow="1770" windowWidth="15555" windowHeight="11820" activeTab="1" xr2:uid="{AFE0E111-50F6-4B5C-96FF-CA711A8C03A0}"/>
+    <workbookView xWindow="660" yWindow="660" windowWidth="17010" windowHeight="6375" xr2:uid="{AFE0E111-50F6-4B5C-96FF-CA711A8C03A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L9"/>
+  <oleSize ref="A1:K9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Address1</t>
   </si>
@@ -42,9 +42,6 @@
     <t>PatientFirstName</t>
   </si>
   <si>
-    <t>MobileNumber </t>
-  </si>
-  <si>
     <t>EmailId</t>
   </si>
   <si>
@@ -99,17 +96,52 @@
     <t>santhos@gmail.com</t>
   </si>
   <si>
-    <t>venkateshtitaniumhq@gmail.com</t>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Dindigul</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>patienttype</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Heart</t>
+  </si>
+  <si>
+    <t>Outpatient</t>
+  </si>
+  <si>
+    <t>Inpatient</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="00000"/>
-    <numFmt numFmtId="165" formatCode="0_);\(0\)"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -180,31 +212,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -520,355 +569,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F83158-9B43-44D4-91C8-3E505B2B7A88}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="13" customWidth="1"/>
+    <col min="2" max="3" width="17.28515625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="19" customWidth="1"/>
+    <col min="5" max="7" width="17" style="19" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="13"/>
+    <col min="9" max="9" width="11.140625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="13" customWidth="1"/>
+    <col min="11" max="13" width="9.140625" style="13"/>
+    <col min="14" max="14" width="13.140625" style="19" customWidth="1"/>
+    <col min="15" max="15" width="19.85546875" style="13" customWidth="1"/>
+    <col min="16" max="16" width="16" style="19" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1">
+    <row r="1" spans="1:18" s="10" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="M1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="P1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="Q1" s="9"/>
+    </row>
+    <row r="2" spans="1:18" s="11" customFormat="1">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="7"/>
-    </row>
-    <row r="2" spans="1:12" s="12" customFormat="1">
-      <c r="A2" s="9" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="17">
+        <v>5301995</v>
+      </c>
+      <c r="E2" s="17">
+        <v>6465646541</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="13">
-        <v>65464654654</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="I2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="17">
+        <v>555555</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="M2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="17">
+        <v>7010911215</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="17">
+        <v>5555555555</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="12" customFormat="1">
+      <c r="A3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="7">
+        <v>12281995</v>
+      </c>
+      <c r="E3" s="7">
+        <v>5456456</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="6">
+        <v>6465</v>
+      </c>
+      <c r="J3" s="6">
+        <v>68468464</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="10">
-        <v>555555</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="9">
-        <v>7010911215</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="9">
-        <v>5555555555</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="3">
-        <v>5456456</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="M3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="7">
+        <v>707070707070</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="3">
-        <v>6465</v>
-      </c>
-      <c r="F3" s="3">
-        <v>68468464</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="5">
-        <v>707070707070</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="3">
+      <c r="P3" s="7">
         <v>54545454554</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
+    <row r="4" spans="1:18" s="13" customFormat="1">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="P4" s="19"/>
+    </row>
+    <row r="5" spans="1:18" s="13" customFormat="1">
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="P5" s="19"/>
+    </row>
+    <row r="6" spans="1:18" s="13" customFormat="1">
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="P6" s="19"/>
+    </row>
+    <row r="7" spans="1:18" s="13" customFormat="1">
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="P7" s="19"/>
+    </row>
+    <row r="8" spans="1:18" s="13" customFormat="1">
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="P8" s="19"/>
+    </row>
+    <row r="9" spans="1:18" s="13" customFormat="1">
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="P9" s="19"/>
+    </row>
+    <row r="10" spans="1:18" s="13" customFormat="1">
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="P10" s="19"/>
+    </row>
+    <row r="11" spans="1:18" s="13" customFormat="1">
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="P11" s="19"/>
+    </row>
+    <row r="12" spans="1:18" s="13" customFormat="1">
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="P12" s="19"/>
+    </row>
+    <row r="13" spans="1:18" s="13" customFormat="1">
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="P13" s="19"/>
+    </row>
+    <row r="14" spans="1:18" s="13" customFormat="1">
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="P14" s="19"/>
+    </row>
+    <row r="15" spans="1:18" s="13" customFormat="1">
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="P15" s="19"/>
+    </row>
+    <row r="16" spans="1:18" s="13" customFormat="1">
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="P16" s="19"/>
+    </row>
+    <row r="17" spans="1:18" s="13" customFormat="1">
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="P17" s="19"/>
+    </row>
+    <row r="18" spans="1:18" s="13" customFormat="1">
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="P18" s="19"/>
+    </row>
+    <row r="19" spans="1:18" s="13" customFormat="1">
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="P19" s="19"/>
+    </row>
+    <row r="20" spans="1:18" s="13" customFormat="1">
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="P20" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{06130636-9BB1-4687-8033-AFFF35C922EB}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{CB031BCC-555D-4D65-A3F5-40182B3CDDB5}"/>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{06130636-9BB1-4687-8033-AFFF35C922EB}"/>
+    <hyperlink ref="O3" r:id="rId2" xr:uid="{CB031BCC-555D-4D65-A3F5-40182B3CDDB5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -879,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{312B01E5-AB42-4A96-8372-073F147C4E5A}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -890,29 +903,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="3" spans="1:2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{17254089-B9D1-4D08-99A8-3E0403E254CF}"/>

</xml_diff>